<commit_message>
Latest Pages and Test cases has been added and pushed
</commit_message>
<xml_diff>
--- a/com.att/TestData/NewData.xlsx
+++ b/com.att/TestData/NewData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>SLID</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>Demo39812qq</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>256 GB</t>
   </si>
 </sst>
 </file>
@@ -367,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -395,6 +401,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>